<commit_message>
Commit final antes de alternar para a main
</commit_message>
<xml_diff>
--- a/SOLICITACOES_AUTORIZACAO_FACPLAN.xlsx
+++ b/SOLICITACOES_AUTORIZACAO_FACPLAN.xlsx
@@ -874,41 +874,14 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>ERRO</t>
+          <t>8352488</t>
         </is>
       </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Erro ao salvar e confirmar: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=129.0.6668.90)
-Stacktrace:
-	GetHandleVerifier [0x00007FF6DAB5B095+29557]
-	(No symbol) [0x00007FF6DAACFA50]
-	(No symbol) [0x00007FF6DA98B56A]
-	(No symbol) [0x00007FF6DA95FCC5]
-	(No symbol) [0x00007FF6DAA0EE07]
-	(No symbol) [0x00007FF6DAA27E21]
-	(No symbol) [0x00007FF6DAA06F33]
-	(No symbol) [0x00007FF6DA9D116F]
-	(No symbol) [0x00007FF6DA9D22D1]
-	GetHandleVerifier [0x00007FF6DAE8C96D+3378253]
-	GetHandleVerifier [0x00007FF6DAED8497+3688311]
-	GetHandleVerifier [0x00007FF6DAECD1CB+3642539]
-	GetHandleVerifier [0x00007FF6DAC1A6B6+813462]
-	(No symbol) [0x00007FF6DAADAB5F]
-	(No symbol) [0x00007FF6DAAD6B74]
-	(No symbol) [0x00007FF6DAAD6D10]
-	(No symbol) [0x00007FF6DAAC5C1F]
-	BaseThreadInitThunk [0x00007FF9619C257D+29]
-	RtlUserThreadStart [0x00007FF963C4AF08+40]
-</t>
-        </is>
-      </c>
+      <c r="T6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -971,12 +944,20 @@
           <t xml:space="preserve">AUTORIZAÇÃO MENSAL  - Relativo atendimentos do período 16/09/2024 a 30/09/2024  anexo relatório médico e relatório Clínico, </t>
         </is>
       </c>
-      <c r="O7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>ERRO</t>
+        </is>
+      </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Erro na função process_row</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">

</xml_diff>